<commit_message>
chore: update final evaluation benchmark data
Fixed wrong Gemini-3.5 name in GPT-5.2 final evaluation data
</commit_message>
<xml_diff>
--- a/data/benchmarks/final_evaluation.xlsx
+++ b/data/benchmarks/final_evaluation.xlsx
@@ -306,15 +306,12 @@
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="6" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -327,12 +324,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="2" fillId="7" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="8" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="8" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -868,7 +859,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="I16" zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="87" workbookViewId="0">
       <selection activeCell="P27" activeCellId="0" sqref="P27"/>
     </sheetView>
   </sheetViews>
@@ -1017,7 +1008,7 @@
       <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="1"/>
@@ -1031,14 +1022,14 @@
       <c r="N6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1052,28 +1043,28 @@
       <c r="H7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1087,28 +1078,28 @@
       <c r="H8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1122,28 +1113,28 @@
       <c r="H9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1193,248 +1184,248 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" ht="27.600000000000001" customHeight="1">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="M13" s="1"/>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="Q13" s="7" t="s">
+      <c r="Q13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="R13" s="8" t="s">
+      <c r="R13" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" ht="27.600000000000001" customHeight="1">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>4</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="7" t="s">
+      <c r="N14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="8" t="s">
+      <c r="O14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="P14" s="1"/>
-      <c r="Q14" s="7" t="s">
+      <c r="Q14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="R14" s="8" t="s">
+      <c r="R14" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" ht="28.199999999999999" customHeight="1">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="7" t="s">
         <v>31</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="M15" s="1"/>
-      <c r="N15" s="7" t="s">
+      <c r="N15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O15" s="10" t="s">
+      <c r="O15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="P15" s="1"/>
-      <c r="Q15" s="7" t="s">
+      <c r="Q15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R15" s="10" t="s">
+      <c r="R15" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="7" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="7" t="s">
         <v>35</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="7" t="s">
+      <c r="N16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="7" t="s">
         <v>36</v>
       </c>
       <c r="P16" s="1"/>
-      <c r="Q16" s="7" t="s">
+      <c r="Q16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R16" s="10" t="s">
+      <c r="R16" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" ht="30.600000000000001" customHeight="1">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="7" t="s">
         <v>31</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="7" t="s">
+      <c r="K17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="7" t="s">
         <v>10</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="7" t="s">
+      <c r="N17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="O17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="P17" s="1"/>
-      <c r="Q17" s="7" t="s">
+      <c r="Q17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="R17" s="10" t="s">
+      <c r="R17" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" ht="29.399999999999999" customHeight="1">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="7" t="s">
         <v>39</v>
       </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="7" t="s">
+      <c r="K18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="7" t="s">
         <v>40</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="7" t="s">
+      <c r="N18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="O18" s="10" t="s">
+      <c r="O18" s="7" t="s">
         <v>41</v>
       </c>
       <c r="P18" s="1"/>
-      <c r="Q18" s="7" t="s">
+      <c r="Q18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R18" s="10" t="s">
+      <c r="R18" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1484,212 +1475,212 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" ht="30" customHeight="1">
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="9" t="s">
         <v>43</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="L22" s="9" t="s">
         <v>43</v>
       </c>
       <c r="M22" s="1"/>
-      <c r="N22" s="11" t="s">
+      <c r="N22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="O22" s="12" t="s">
+      <c r="O22" s="9" t="s">
         <v>43</v>
       </c>
       <c r="P22" s="1"/>
-      <c r="Q22" s="11" t="s">
+      <c r="Q22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="R22" s="12" t="s">
+      <c r="R22" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" ht="31.800000000000001" customHeight="1">
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>3</v>
+      <c r="I23" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L23" s="12" t="s">
+      <c r="L23" s="9" t="s">
         <v>5</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="11" t="s">
+      <c r="N23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="O23" s="12" t="s">
+      <c r="O23" s="9" t="s">
         <v>6</v>
       </c>
       <c r="P23" s="1"/>
-      <c r="Q23" s="11" t="s">
+      <c r="Q23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="R23" s="12" t="s">
+      <c r="R23" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" ht="29.399999999999999" customHeight="1">
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="9" t="s">
         <v>45</v>
       </c>
       <c r="J24" s="1"/>
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="L24" s="9" t="s">
         <v>46</v>
       </c>
       <c r="M24" s="1"/>
-      <c r="N24" s="11" t="s">
+      <c r="N24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O24" s="13" t="s">
+      <c r="O24" s="9" t="s">
         <v>47</v>
       </c>
       <c r="P24" s="1"/>
-      <c r="Q24" s="11" t="s">
+      <c r="Q24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="R24" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" ht="30.600000000000001" customHeight="1">
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="I25" s="9" t="s">
         <v>50</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="L25" s="9" t="s">
         <v>51</v>
       </c>
       <c r="M25" s="1"/>
-      <c r="N25" s="11" t="s">
+      <c r="N25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O25" s="13" t="s">
+      <c r="O25" s="9" t="s">
         <v>52</v>
       </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="11" t="s">
+      <c r="Q25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="R25" s="13" t="s">
+      <c r="R25" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" ht="28.199999999999999" customHeight="1">
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="9" t="s">
         <v>45</v>
       </c>
       <c r="J26" s="1"/>
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="13" t="s">
+      <c r="L26" s="9" t="s">
         <v>46</v>
       </c>
       <c r="M26" s="1"/>
-      <c r="N26" s="11" t="s">
+      <c r="N26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O26" s="13" t="s">
+      <c r="O26" s="9" t="s">
         <v>47</v>
       </c>
       <c r="P26" s="1"/>
-      <c r="Q26" s="11" t="s">
+      <c r="Q26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="13" t="s">
+      <c r="R26" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" ht="28.199999999999999" customHeight="1">
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="I27" s="9" t="s">
         <v>55</v>
       </c>
       <c r="J27" s="1"/>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="13" t="s">
+      <c r="L27" s="9" t="s">
         <v>56</v>
       </c>
       <c r="M27" s="1"/>
-      <c r="N27" s="11" t="s">
+      <c r="N27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="13" t="s">
+      <c r="O27" s="9" t="s">
         <v>57</v>
       </c>
       <c r="P27" s="1"/>
-      <c r="Q27" s="11" t="s">
+      <c r="Q27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="R27" s="13" t="s">
+      <c r="R27" s="9" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>